<commit_message>
Add the function get_unique
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiley/Documents/RbiMs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816EE9F7-DE86-5D4F-BF10-8D790580C2B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFF275C-DCB9-DE44-973B-2CCD6B86271B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21040" yWindow="1220" windowWidth="17480" windowHeight="14080" xr2:uid="{A5F320E3-CED3-2644-A86A-2708247163D3}"/>
+    <workbookView xWindow="-29600" yWindow="1220" windowWidth="26040" windowHeight="14080" xr2:uid="{A5F320E3-CED3-2644-A86A-2708247163D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,21 +54,9 @@
     <t>Bin_2</t>
   </si>
   <si>
-    <t>Sample site</t>
-  </si>
-  <si>
-    <t>Bin name</t>
-  </si>
-  <si>
-    <t>Stuary</t>
-  </si>
-  <si>
     <t>Sediment4</t>
   </si>
   <si>
-    <t>Water column</t>
-  </si>
-  <si>
     <t>Domain</t>
   </si>
   <si>
@@ -156,13 +144,25 @@
     <t>Clades</t>
   </si>
   <si>
-    <t>Clade 1</t>
-  </si>
-  <si>
-    <t>Clade 2</t>
-  </si>
-  <si>
-    <t>Clade 3</t>
+    <t>Bin_name</t>
+  </si>
+  <si>
+    <t>Sample_site</t>
+  </si>
+  <si>
+    <t>Etuary</t>
+  </si>
+  <si>
+    <t>Water_column</t>
+  </si>
+  <si>
+    <t>Clade_1</t>
+  </si>
+  <si>
+    <t>Clade_2</t>
+  </si>
+  <si>
+    <t>Clade_3</t>
   </si>
 </sst>
 </file>
@@ -534,44 +534,46 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
     <col min="10" max="10" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -579,31 +581,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -611,31 +613,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -643,31 +645,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>42</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -675,31 +677,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
         <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -707,31 +709,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -739,31 +741,31 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>